<commit_message>
New version of the LIXDC with Sample Manager and HPLC Data Collection
</commit_message>
<xml_diff>
--- a/util/Sample_Import.xlsx
+++ b/util/Sample_Import.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="54380" yWindow="640" windowWidth="25600" windowHeight="27540" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>X</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Temperature ( C )</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>96wp</t>
   </si>
 </sst>
 </file>
@@ -556,479 +562,487 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="4"/>
-      <c r="C1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1">
         <v>1000000000001</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" t="str">
-        <f>CONCATENATE("Sample Imp ",C3,"-",D3)</f>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="str">
+        <f>CONCATENATE("Sample Imp ",D3,"-",E3)</f>
         <v>Sample Imp 1-1</v>
       </c>
-      <c r="F3" t="str">
-        <f>CONCATENATE("S",C3,"-",D3)</f>
+      <c r="G3" t="str">
+        <f>CONCATENATE("S",D3,"-",E3)</f>
         <v>S1-1</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.77500000000000002</v>
       </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
       <c r="I3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>2</v>
       </c>
-      <c r="E4" t="str">
-        <f>CONCATENATE("Sample Imp ",C4,"-",D4)</f>
+      <c r="F4" t="str">
+        <f>CONCATENATE("Sample Imp ",D4,"-",E4)</f>
         <v>Sample Imp 1-2</v>
       </c>
-      <c r="F4" t="str">
-        <f t="shared" ref="F4:F18" si="0">CONCATENATE("S",C4,"-",D4)</f>
+      <c r="G4" t="str">
+        <f t="shared" ref="G4:G18" si="0">CONCATENATE("S",D4,"-",E4)</f>
         <v>S1-2</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.77200000000000002</v>
       </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
       <c r="I4">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>3</v>
       </c>
-      <c r="E5" t="str">
-        <f t="shared" ref="E5:E18" si="1">CONCATENATE("Sample Imp ",C5,"-",D5)</f>
+      <c r="F5" t="str">
+        <f t="shared" ref="F5:F18" si="1">CONCATENATE("Sample Imp ",D5,"-",E5)</f>
         <v>Sample Imp 1-3</v>
       </c>
-      <c r="F5" t="str">
+      <c r="G5" t="str">
         <f t="shared" si="0"/>
         <v>S1-3</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.77600000000000002</v>
       </c>
-      <c r="H5">
-        <v>10</v>
-      </c>
       <c r="I5">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="D6">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>4</v>
       </c>
-      <c r="E6" t="str">
+      <c r="F6" t="str">
         <f t="shared" si="1"/>
         <v>Sample Imp 1-4</v>
       </c>
-      <c r="F6" t="str">
+      <c r="G6" t="str">
         <f t="shared" si="0"/>
         <v>S1-4</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.47499999999999998</v>
       </c>
-      <c r="H6">
-        <v>10</v>
-      </c>
       <c r="I6">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="D7">
         <v>1</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>5</v>
       </c>
-      <c r="E7" t="str">
+      <c r="F7" t="str">
         <f t="shared" si="1"/>
         <v>Sample Imp 1-5</v>
       </c>
-      <c r="F7" t="str">
+      <c r="G7" t="str">
         <f t="shared" si="0"/>
         <v>S1-5</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0.441</v>
       </c>
-      <c r="H7">
-        <v>10</v>
-      </c>
       <c r="I7">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="D8">
         <v>1</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>6</v>
       </c>
-      <c r="E8" t="str">
+      <c r="F8" t="str">
         <f t="shared" si="1"/>
         <v>Sample Imp 1-6</v>
       </c>
-      <c r="F8" t="str">
+      <c r="G8" t="str">
         <f t="shared" si="0"/>
         <v>S1-6</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0.78800000000000003</v>
       </c>
-      <c r="H8">
-        <v>10</v>
-      </c>
       <c r="I8">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="D9">
         <v>1</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>7</v>
       </c>
-      <c r="E9" t="str">
+      <c r="F9" t="str">
         <f t="shared" si="1"/>
         <v>Sample Imp 1-7</v>
       </c>
-      <c r="F9" t="str">
+      <c r="G9" t="str">
         <f t="shared" si="0"/>
         <v>S1-7</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>0.95799999999999996</v>
       </c>
-      <c r="H9">
-        <v>10</v>
-      </c>
       <c r="I9">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="D10">
         <v>1</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>8</v>
       </c>
-      <c r="E10" t="str">
+      <c r="F10" t="str">
         <f t="shared" si="1"/>
         <v>Sample Imp 1-8</v>
       </c>
-      <c r="F10" t="str">
+      <c r="G10" t="str">
         <f t="shared" si="0"/>
         <v>S1-8</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0.48</v>
       </c>
-      <c r="H10">
-        <v>10</v>
-      </c>
       <c r="I10">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="J10">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="D11">
         <v>2</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1</v>
       </c>
-      <c r="E11" t="str">
+      <c r="F11" t="str">
         <f t="shared" si="1"/>
         <v>Sample Imp 2-1</v>
       </c>
-      <c r="F11" t="str">
+      <c r="G11" t="str">
         <f t="shared" si="0"/>
         <v>S2-1</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>0.317</v>
       </c>
-      <c r="H11">
-        <v>10</v>
-      </c>
       <c r="I11">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="C12">
-        <v>2</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="D12">
         <v>2</v>
       </c>
-      <c r="E12" t="str">
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="str">
         <f t="shared" si="1"/>
         <v>Sample Imp 2-2</v>
       </c>
-      <c r="F12" t="str">
+      <c r="G12" t="str">
         <f t="shared" si="0"/>
         <v>S2-2</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>0.45900000000000002</v>
       </c>
-      <c r="H12">
-        <v>10</v>
-      </c>
       <c r="I12">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="D13">
         <v>2</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>3</v>
       </c>
-      <c r="E13" t="str">
+      <c r="F13" t="str">
         <f t="shared" si="1"/>
         <v>Sample Imp 2-3</v>
       </c>
-      <c r="F13" t="str">
+      <c r="G13" t="str">
         <f t="shared" si="0"/>
         <v>S2-3</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>0.248</v>
       </c>
-      <c r="H13">
-        <v>10</v>
-      </c>
       <c r="I13">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="J13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="D14">
         <v>2</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>4</v>
       </c>
-      <c r="E14" t="str">
+      <c r="F14" t="str">
         <f t="shared" si="1"/>
         <v>Sample Imp 2-4</v>
       </c>
-      <c r="F14" t="str">
+      <c r="G14" t="str">
         <f t="shared" si="0"/>
         <v>S2-4</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>0.39</v>
       </c>
-      <c r="H14">
-        <v>10</v>
-      </c>
       <c r="I14">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="J14">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="D15">
         <v>2</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>5</v>
       </c>
-      <c r="E15" t="str">
+      <c r="F15" t="str">
         <f t="shared" si="1"/>
         <v>Sample Imp 2-5</v>
       </c>
-      <c r="F15" t="str">
+      <c r="G15" t="str">
         <f t="shared" si="0"/>
         <v>S2-5</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>0.57399999999999995</v>
       </c>
-      <c r="H15">
-        <v>10</v>
-      </c>
       <c r="I15">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="J15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="D16">
         <v>2</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>6</v>
       </c>
-      <c r="E16" t="str">
+      <c r="F16" t="str">
         <f t="shared" si="1"/>
         <v>Sample Imp 2-6</v>
       </c>
-      <c r="F16" t="str">
+      <c r="G16" t="str">
         <f t="shared" si="0"/>
         <v>S2-6</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>0.79900000000000004</v>
       </c>
-      <c r="H16">
-        <v>10</v>
-      </c>
       <c r="I16">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="3:9">
-      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="J16">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10">
+      <c r="D17">
         <v>2</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>7</v>
       </c>
-      <c r="E17" t="str">
+      <c r="F17" t="str">
         <f t="shared" si="1"/>
         <v>Sample Imp 2-7</v>
       </c>
-      <c r="F17" t="str">
+      <c r="G17" t="str">
         <f t="shared" si="0"/>
         <v>S2-7</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>0.371</v>
       </c>
-      <c r="H17">
-        <v>10</v>
-      </c>
       <c r="I17">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9">
-      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="J17">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10">
+      <c r="D18">
         <v>2</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>8</v>
       </c>
-      <c r="E18" t="str">
+      <c r="F18" t="str">
         <f t="shared" si="1"/>
         <v>Sample Imp 2-8</v>
       </c>
-      <c r="F18" t="str">
+      <c r="G18" t="str">
         <f t="shared" si="0"/>
         <v>S2-8</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="H18">
-        <v>10</v>
-      </c>
       <c r="I18">
+        <v>10</v>
+      </c>
+      <c r="J18">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:J1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>